<commit_message>
update brochure file link address
</commit_message>
<xml_diff>
--- a/brochures/excel/offshore/region-1/AIBT.xlsx
+++ b/brochures/excel/offshore/region-1/AIBT.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zelon\Documents\Code\ViskeeConsultancy\Viskee-Consultancy-Configuration\brochures\excel\offshore\seapae\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zelon\Documents\Code\ViskeeConsultancy\Viskee-Consultancy-Configuration\brochures\excel\offshore\region-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="-105" windowWidth="22140" windowHeight="13170"/>
+    <workbookView xWindow="2895" yWindow="-105" windowWidth="22140" windowHeight="13170"/>
   </bookViews>
   <sheets>
     <sheet name="promotions" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,15 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>https://github.com/Viskee-Consultancy/Viskee-Consultancy-Configuration/raw/master/brochures/pdf/offshore/seapae/aibt/AIBT_Courses_Fees_2021_VOL_2.2.pdf</t>
+    <t>AIBT Region1(SEAPAE) Q4 Promotion.pdf</t>
+  </si>
+  <si>
+    <t>https://github.com/Viskee-Consultancy/Viskee-Consultancy-Configuration/raw/master/brochures/pdf/offshore/region-1/aibt/AIBTSEAPAE_Q4_Brochure_1OCT-31DEC21_VOL1.1.pdf</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>AIBT Region1(SEAPAE) Q4 Promotion.pdf</t>
-  </si>
-  <si>
-    <t>https://github.com/Viskee-Consultancy/Viskee-Consultancy-Configuration/raw/master/brochures/pdf/offshore/seapae/aibt/AIBTSEAPAE_Q4_Brochure_1OCT-31DEC21_VOL1.1.pdf</t>
+    <t>https://github.com/Viskee-Consultancy/Viskee-Consultancy-Configuration/raw/master/brochures/pdf/offshore/region-1/aibt/AIBT_Courses_Fees_2021_VOL_2.2.pdf</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -393,7 +394,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -415,23 +416,24 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update brochure excel files
</commit_message>
<xml_diff>
--- a/brochures/excel/offshore/region-1/AIBT.xlsx
+++ b/brochures/excel/offshore/region-1/AIBT.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="-105" windowWidth="22140" windowHeight="13170"/>
+    <workbookView xWindow="3840" yWindow="-105" windowWidth="22140" windowHeight="13170"/>
   </bookViews>
   <sheets>
-    <sheet name="promotions" sheetId="1" r:id="rId1"/>
+    <sheet name="brochures" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>

</xml_diff>